<commit_message>
Initials checking added, some resourses updated, minor fixes
</commit_message>
<xml_diff>
--- a/resources/names.xlsx
+++ b/resources/names.xlsx
@@ -19,68 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>Александр Альфонс</t>
-  </si>
-  <si>
-    <t>Александр Бродский</t>
-  </si>
-  <si>
-    <t>Александр Васильев</t>
-  </si>
-  <si>
-    <t>Александр Горький</t>
-  </si>
-  <si>
-    <t>Александр Гюго</t>
-  </si>
-  <si>
-    <t>Александр Махонин</t>
-  </si>
-  <si>
-    <t>Александр Роулинг</t>
-  </si>
-  <si>
-    <t>Александр Шоу</t>
-  </si>
-  <si>
-    <t>Алексей Володин</t>
-  </si>
-  <si>
-    <t>Алексей Евгеньевич Блажник</t>
-  </si>
-  <si>
     <t>Аликина Анна</t>
   </si>
   <si>
-    <t>Амелия Ведищева</t>
-  </si>
-  <si>
-    <t>Анастасия Толстова</t>
-  </si>
-  <si>
-    <t>Андрей Багрицкий</t>
-  </si>
-  <si>
-    <t>Андрей Брэдбери</t>
-  </si>
-  <si>
-    <t>Артем Мандельштам</t>
-  </si>
-  <si>
-    <t>Артем Чуковский</t>
-  </si>
-  <si>
-    <t>Артём Мандельштам</t>
-  </si>
-  <si>
-    <t>Ахматова Александровна Екатерина</t>
-  </si>
-  <si>
     <t>Ахматова Екатерина Вадимовна</t>
   </si>
   <si>
@@ -90,141 +36,51 @@
     <t>Беглова Анастасия</t>
   </si>
   <si>
-    <t>Борисович Александр Хармс</t>
-  </si>
-  <si>
     <t>Бронте Николай</t>
   </si>
   <si>
-    <t>Вадим Белец</t>
-  </si>
-  <si>
-    <t>Виктор Колокольцев</t>
-  </si>
-  <si>
-    <t>Виктор Лем</t>
-  </si>
-  <si>
-    <t>Викторовна Арина Кинг</t>
-  </si>
-  <si>
-    <t>Виталий Владимирович Маяковский</t>
-  </si>
-  <si>
-    <t>Витязев Викторович Андрей</t>
-  </si>
-  <si>
-    <t>Владимирович Брагин Дмитрий</t>
-  </si>
-  <si>
-    <t>Вячеславович Оруэлл Андрей</t>
-  </si>
-  <si>
-    <t>Галина Белая</t>
-  </si>
-  <si>
     <t>Гиппиус Дарья</t>
   </si>
   <si>
-    <t>Григорьевич Максим Шукшин</t>
-  </si>
-  <si>
     <t>Губин Иван</t>
   </si>
   <si>
     <t>Губин Павел</t>
   </si>
   <si>
-    <t>Губинич Красавцев Иван</t>
-  </si>
-  <si>
-    <t>Гумилева Александровна Нина</t>
-  </si>
-  <si>
     <t>Гумилева Екатерина Николаевна</t>
   </si>
   <si>
-    <t>Денис Суворов</t>
-  </si>
-  <si>
     <t>Диккенс Георгий</t>
   </si>
   <si>
-    <t>Евгений Комаров</t>
-  </si>
-  <si>
-    <t>Евгений Критник</t>
-  </si>
-  <si>
-    <t>Евгений Сологуб</t>
-  </si>
-  <si>
-    <t>Екатерина Грязнева</t>
-  </si>
-  <si>
-    <t>Елена Цветаева</t>
-  </si>
-  <si>
     <t>Есенин Сергей</t>
   </si>
   <si>
-    <t>Женя Московская</t>
-  </si>
-  <si>
     <t>Жуковский Кирилл</t>
   </si>
   <si>
-    <t>Илья Волошин</t>
-  </si>
-  <si>
-    <t>Илья Сергеевич Ветров</t>
-  </si>
-  <si>
     <t>Илюхина Мария</t>
   </si>
   <si>
     <t>Инокеньтев Иван</t>
   </si>
   <si>
-    <t>Иосиф Горбанидце</t>
-  </si>
-  <si>
-    <t>Ирина Грибоедова</t>
-  </si>
-  <si>
-    <t>Ирина Уайльд</t>
-  </si>
-  <si>
-    <t>Кафка Александрович Сергей</t>
-  </si>
-  <si>
     <t>Киплинг Дарья</t>
   </si>
   <si>
     <t>Клубничкова Дарья</t>
   </si>
   <si>
-    <t>Кристина Леонтьева</t>
-  </si>
-  <si>
     <t>Критник Игорь</t>
   </si>
   <si>
-    <t>Ксения Макродченко</t>
-  </si>
-  <si>
-    <t>Ксения Чехова</t>
-  </si>
-  <si>
     <t>Леонтьев Виктор</t>
   </si>
   <si>
     <t>Леонтьев Сергей</t>
   </si>
   <si>
-    <t>Леонтьевна Генадьенко Татьяна</t>
-  </si>
-  <si>
     <t>Лермонтов Кирилл</t>
   </si>
   <si>
@@ -234,18 +90,6 @@
     <t>Лондон Андрей</t>
   </si>
   <si>
-    <t>Максим Некрасов</t>
-  </si>
-  <si>
-    <t>Маргарита Роллан</t>
-  </si>
-  <si>
-    <t>Марина Архетипова</t>
-  </si>
-  <si>
-    <t>Марк Горбанидце</t>
-  </si>
-  <si>
     <t>Маршак Сергей Владимирович</t>
   </si>
   <si>
@@ -258,51 +102,21 @@
     <t>Московская Евгения</t>
   </si>
   <si>
-    <t>Надежда Брюсова</t>
-  </si>
-  <si>
     <t>Незнаева Александра</t>
   </si>
   <si>
-    <t>Павел Толстой</t>
-  </si>
-  <si>
-    <t>Павел Шершнев</t>
-  </si>
-  <si>
     <t>Пастернак Роман</t>
   </si>
   <si>
-    <t>Паша Брежнев</t>
-  </si>
-  <si>
     <t>Пирогова Екатерина</t>
   </si>
   <si>
     <t>Плавцова Анна</t>
   </si>
   <si>
-    <t>Полина Белая</t>
-  </si>
-  <si>
-    <t>Пушкин Иванович Валерий</t>
-  </si>
-  <si>
     <t>Рейм Мария</t>
   </si>
   <si>
-    <t>Роман Самохвалов</t>
-  </si>
-  <si>
-    <t>Роман Черный</t>
-  </si>
-  <si>
-    <t>Сергей Меринов</t>
-  </si>
-  <si>
-    <t>Сергей Петунин</t>
-  </si>
-  <si>
     <t>Страдальцев Георгий</t>
   </si>
   <si>
@@ -312,15 +126,9 @@
     <t>Сугробов Евгений</t>
   </si>
   <si>
-    <t>Татьяна Леонтьева</t>
-  </si>
-  <si>
     <t>Твен Василий</t>
   </si>
   <si>
-    <t>Теодор Драйзер</t>
-  </si>
-  <si>
     <t>Тэффи Анастасия</t>
   </si>
   <si>
@@ -330,18 +138,9 @@
     <t>Усова Полина</t>
   </si>
   <si>
-    <t>Федорович Андрей Островский</t>
-  </si>
-  <si>
-    <t>Фёдор Гумилев</t>
-  </si>
-  <si>
     <t>Хемингуэй Дмитрий</t>
   </si>
   <si>
-    <t>Хлебников Александер</t>
-  </si>
-  <si>
     <t>Хлебников Александр</t>
   </si>
   <si>
@@ -354,19 +153,208 @@
     <t>Щукин Василий</t>
   </si>
   <si>
-    <t>Эльвира Гоголь</t>
-  </si>
-  <si>
-    <t>Юлия Лесова</t>
-  </si>
-  <si>
     <t>Юлия Манн</t>
   </si>
   <si>
-    <t>Юля Лесова</t>
-  </si>
-  <si>
-    <t>Юрий Гарсиа</t>
+    <t>Альфонс Александр</t>
+  </si>
+  <si>
+    <t>Бродский Александр</t>
+  </si>
+  <si>
+    <t>Васильев Александр</t>
+  </si>
+  <si>
+    <t>Горький Александр</t>
+  </si>
+  <si>
+    <t>Гюго Александр</t>
+  </si>
+  <si>
+    <t>Махонин Александр</t>
+  </si>
+  <si>
+    <t>Роулинг Александр</t>
+  </si>
+  <si>
+    <t>Шоу Александр</t>
+  </si>
+  <si>
+    <t>Володин Алексей</t>
+  </si>
+  <si>
+    <t>Блажник Алексей Евгеньевич</t>
+  </si>
+  <si>
+    <t>Ведищева Амелия</t>
+  </si>
+  <si>
+    <t>Толстова Анастасия</t>
+  </si>
+  <si>
+    <t>Багрицкий Андрей</t>
+  </si>
+  <si>
+    <t>Брэдбери Андрей</t>
+  </si>
+  <si>
+    <t>Мандельштам Артем</t>
+  </si>
+  <si>
+    <t>Чуковский Артем</t>
+  </si>
+  <si>
+    <t>Ахматова Екатерина Александровна</t>
+  </si>
+  <si>
+    <t>Хармс Александр Борисович</t>
+  </si>
+  <si>
+    <t>Витязев Андрей Викторович</t>
+  </si>
+  <si>
+    <t>Маяковский Виталий Владимирович</t>
+  </si>
+  <si>
+    <t>Кинг Арина Викторовна</t>
+  </si>
+  <si>
+    <t>Лем Виктор</t>
+  </si>
+  <si>
+    <t>Колокольцев Виктор</t>
+  </si>
+  <si>
+    <t>Белец Вадим</t>
+  </si>
+  <si>
+    <t>Брагин Владимирович Дмитрий</t>
+  </si>
+  <si>
+    <t>Оруэлл Андрей Вячеславович</t>
+  </si>
+  <si>
+    <t>Белая Галина</t>
+  </si>
+  <si>
+    <t>Шукшин Максим Григорьевич</t>
+  </si>
+  <si>
+    <t>Красавцев Иван Губинич</t>
+  </si>
+  <si>
+    <t>Гумилева Нина Александровна</t>
+  </si>
+  <si>
+    <t>Суворов Денис</t>
+  </si>
+  <si>
+    <t>Комаров Евгений</t>
+  </si>
+  <si>
+    <t>Критник Евгений</t>
+  </si>
+  <si>
+    <t>Сологуб Евгений</t>
+  </si>
+  <si>
+    <t>Грязнева Екатерина</t>
+  </si>
+  <si>
+    <t>Цветаева Елена</t>
+  </si>
+  <si>
+    <t>Волошин Илья</t>
+  </si>
+  <si>
+    <t>Ветров Илья Сергеевич</t>
+  </si>
+  <si>
+    <t>Горбанидце Иосиф</t>
+  </si>
+  <si>
+    <t>Грибоедова Ирина</t>
+  </si>
+  <si>
+    <t>Уайльд Ирина</t>
+  </si>
+  <si>
+    <t>Кафка Сергей Александрович</t>
+  </si>
+  <si>
+    <t>Леонтьева Кристина</t>
+  </si>
+  <si>
+    <t>Макродченко Ксения</t>
+  </si>
+  <si>
+    <t>Чехова Ксения</t>
+  </si>
+  <si>
+    <t>Генадьенко Татьяна Леонтьевна</t>
+  </si>
+  <si>
+    <t>Некрасов Максим</t>
+  </si>
+  <si>
+    <t>Роллан Маргарита</t>
+  </si>
+  <si>
+    <t>Архетипова Марина</t>
+  </si>
+  <si>
+    <t>Горбанидце Марк</t>
+  </si>
+  <si>
+    <t>Брюсова Надежда</t>
+  </si>
+  <si>
+    <t>Толстой Павел</t>
+  </si>
+  <si>
+    <t>Шершнев Павел</t>
+  </si>
+  <si>
+    <t>Брежнев Паша</t>
+  </si>
+  <si>
+    <t>Белая Полина</t>
+  </si>
+  <si>
+    <t>Пушкин Валерий Иванович</t>
+  </si>
+  <si>
+    <t>Самохвалов Роман</t>
+  </si>
+  <si>
+    <t>Черный Роман</t>
+  </si>
+  <si>
+    <t>Меринов Сергей</t>
+  </si>
+  <si>
+    <t>Петунин Сергей</t>
+  </si>
+  <si>
+    <t>Леонтьева Татьяна</t>
+  </si>
+  <si>
+    <t>Драйзер Теодор</t>
+  </si>
+  <si>
+    <t>Островский Андрей Федорович</t>
+  </si>
+  <si>
+    <t>Гумилев Фёдор</t>
+  </si>
+  <si>
+    <t>Гоголь Эльвира</t>
+  </si>
+  <si>
+    <t>Лесова Юлия</t>
+  </si>
+  <si>
+    <t>Гарсиа Юрий</t>
   </si>
 </sst>
 </file>
@@ -432,6 +420,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -449,20 +451,6 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -477,8 +465,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:A116" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:A116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:A112" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:A112"/>
+  <sortState ref="A2:A112">
+    <sortCondition ref="A112"/>
+  </sortState>
   <tableColumns count="1">
     <tableColumn id="1" name="name"/>
   </tableColumns>
@@ -771,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A116"/>
+  <dimension ref="A1:A112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,502 +785,502 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
@@ -1299,67 +1290,47 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>